<commit_message>
first working model for LAFPP
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -1351,14 +1351,14 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2757,8 +2757,8 @@
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="160"/>
-      <c r="V7" s="160"/>
+      <c r="U7" s="161"/>
+      <c r="V7" s="161"/>
       <c r="W7" s="12"/>
       <c r="X7" s="109"/>
       <c r="Y7" s="109"/>
@@ -6684,16 +6684,16 @@
       <c r="B6" s="147" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="162" t="s">
+      <c r="C6" s="160" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="162" t="s">
+      <c r="D6" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="162" t="s">
+      <c r="E6" s="160" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="162" t="s">
+      <c r="F6" s="160" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6701,16 +6701,16 @@
       <c r="B7" s="147" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="162">
+      <c r="C7" s="160">
         <v>1</v>
       </c>
-      <c r="D7" s="162">
+      <c r="D7" s="160">
         <v>1</v>
       </c>
-      <c r="E7" s="162">
+      <c r="E7" s="160">
         <v>0</v>
       </c>
-      <c r="F7" s="162">
+      <c r="F7" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6718,16 +6718,16 @@
       <c r="B8" s="147" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="162">
+      <c r="C8" s="160">
         <v>13</v>
       </c>
-      <c r="D8" s="162">
+      <c r="D8" s="160">
         <v>9</v>
       </c>
-      <c r="E8" s="162">
+      <c r="E8" s="160">
         <v>0</v>
       </c>
-      <c r="F8" s="162">
+      <c r="F8" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6735,16 +6735,16 @@
       <c r="B9" s="147" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="162">
+      <c r="C9" s="160">
         <v>28</v>
       </c>
-      <c r="D9" s="162">
+      <c r="D9" s="160">
         <v>808</v>
       </c>
-      <c r="E9" s="162">
+      <c r="E9" s="160">
         <v>0</v>
       </c>
-      <c r="F9" s="162">
+      <c r="F9" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6752,16 +6752,16 @@
       <c r="B10" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="160">
         <v>55</v>
       </c>
-      <c r="D10" s="162">
+      <c r="D10" s="160">
         <v>268</v>
       </c>
-      <c r="E10" s="162">
+      <c r="E10" s="160">
         <v>0</v>
       </c>
-      <c r="F10" s="162">
+      <c r="F10" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6769,16 +6769,16 @@
       <c r="B11" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="162">
+      <c r="C11" s="160">
         <v>2894</v>
       </c>
-      <c r="D11" s="162">
+      <c r="D11" s="160">
         <v>7675</v>
       </c>
-      <c r="E11" s="162">
+      <c r="E11" s="160">
         <v>103</v>
       </c>
-      <c r="F11" s="162">
+      <c r="F11" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6786,16 +6786,16 @@
       <c r="B12" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="C12" s="162">
+      <c r="C12" s="160">
         <v>146</v>
       </c>
-      <c r="D12" s="162">
+      <c r="D12" s="160">
         <v>1057</v>
       </c>
-      <c r="E12" s="162">
+      <c r="E12" s="160">
         <v>12</v>
       </c>
-      <c r="F12" s="162">
+      <c r="F12" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6846,16 +6846,16 @@
       <c r="A6" s="147" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="160" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="162" t="s">
+      <c r="C6" s="160" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="162" t="s">
+      <c r="D6" s="160" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="162" t="s">
+      <c r="E6" s="160" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6863,16 +6863,16 @@
       <c r="A7" s="147" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="162">
+      <c r="B7" s="160">
         <v>1</v>
       </c>
-      <c r="C7" s="162">
+      <c r="C7" s="160">
         <v>1</v>
       </c>
-      <c r="D7" s="162">
+      <c r="D7" s="160">
         <v>0</v>
       </c>
-      <c r="E7" s="162">
+      <c r="E7" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6880,16 +6880,16 @@
       <c r="A8" s="147" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="162">
+      <c r="B8" s="160">
         <v>13</v>
       </c>
-      <c r="C8" s="162">
+      <c r="C8" s="160">
         <v>9</v>
       </c>
-      <c r="D8" s="162">
+      <c r="D8" s="160">
         <v>0</v>
       </c>
-      <c r="E8" s="162">
+      <c r="E8" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6897,16 +6897,16 @@
       <c r="A9" s="147" t="s">
         <v>118</v>
       </c>
-      <c r="B9" s="162">
+      <c r="B9" s="160">
         <v>28</v>
       </c>
-      <c r="C9" s="162">
+      <c r="C9" s="160">
         <v>808</v>
       </c>
-      <c r="D9" s="162">
+      <c r="D9" s="160">
         <v>0</v>
       </c>
-      <c r="E9" s="162">
+      <c r="E9" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6914,16 +6914,16 @@
       <c r="A10" s="147" t="s">
         <v>119</v>
       </c>
-      <c r="B10" s="162">
+      <c r="B10" s="160">
         <v>55</v>
       </c>
-      <c r="C10" s="162">
+      <c r="C10" s="160">
         <v>268</v>
       </c>
-      <c r="D10" s="162">
+      <c r="D10" s="160">
         <v>0</v>
       </c>
-      <c r="E10" s="162">
+      <c r="E10" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6931,16 +6931,16 @@
       <c r="A11" s="147" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="162">
+      <c r="B11" s="160">
         <v>2894</v>
       </c>
-      <c r="C11" s="162">
+      <c r="C11" s="160">
         <v>7675</v>
       </c>
-      <c r="D11" s="162">
+      <c r="D11" s="160">
         <v>103</v>
       </c>
-      <c r="E11" s="162">
+      <c r="E11" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -6948,16 +6948,16 @@
       <c r="A12" s="147" t="s">
         <v>121</v>
       </c>
-      <c r="B12" s="162">
+      <c r="B12" s="160">
         <v>146</v>
       </c>
-      <c r="C12" s="162">
+      <c r="C12" s="160">
         <v>1057</v>
       </c>
-      <c r="D12" s="162">
+      <c r="D12" s="160">
         <v>12</v>
       </c>
-      <c r="E12" s="162">
+      <c r="E12" s="160">
         <v>2015</v>
       </c>
     </row>
@@ -8447,7 +8447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -8566,8 +8566,8 @@
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
-      <c r="V7" s="160"/>
-      <c r="W7" s="160"/>
+      <c r="V7" s="161"/>
+      <c r="W7" s="161"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
@@ -9635,8 +9635,8 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
-      <c r="T6" s="160"/>
-      <c r="U6" s="160"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="161"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
     </row>
@@ -10628,8 +10628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10752,8 +10752,8 @@
       <c r="U7" s="109"/>
       <c r="V7" s="109"/>
       <c r="W7" s="109"/>
-      <c r="X7" s="161"/>
-      <c r="Y7" s="161"/>
+      <c r="X7" s="162"/>
+      <c r="Y7" s="162"/>
       <c r="Z7" s="109"/>
       <c r="AA7" s="109"/>
       <c r="AB7" s="109"/>

</xml_diff>

<commit_message>
update checking death and disability benefit
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -4868,7 +4868,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:C32"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5309,8 +5309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6813,7 +6813,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9563,7 +9563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -10628,8 +10628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12006,7 +12006,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
disability benefit, with simple initial disabled.
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -5309,7 +5309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -5532,7 +5532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -6651,7 +6651,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
simulated distribution of initial retirees
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="11" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Other_t6_noHPP" sheetId="15" r:id="rId17"/>
     <sheet name="Other_t5_HPP" sheetId="16" r:id="rId18"/>
     <sheet name="Other_t6_HPP" sheetId="17" r:id="rId19"/>
+    <sheet name="nonActives_allTiers" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="134">
   <si>
     <t>TOC</t>
   </si>
@@ -647,6 +648,21 @@
   <si>
     <t>F12</t>
   </si>
+  <si>
+    <t>t5_HPP</t>
+  </si>
+  <si>
+    <t>t5_noHPP</t>
+  </si>
+  <si>
+    <t>t6_noHPP</t>
+  </si>
+  <si>
+    <t>t6_HPP</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
 </sst>
 </file>
 
@@ -657,7 +673,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +754,12 @@
       <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -882,7 +904,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1359,6 +1381,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4868,7 +4903,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5087,7 +5122,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5309,8 +5344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5532,8 +5567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5756,7 +5791,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5982,7 +6017,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6205,7 +6240,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6428,7 +6463,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6805,6 +6840,473 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="16" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="24" x14ac:dyDescent="0.25">
+      <c r="B6" s="163" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="164" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="164" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="164" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="164" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="164" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="164" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="164" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="164" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="164" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="164" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="164" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="164" t="s">
+        <v>110</v>
+      </c>
+      <c r="O6" s="164" t="s">
+        <v>111</v>
+      </c>
+      <c r="P6" s="164" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="167" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="165">
+        <v>0</v>
+      </c>
+      <c r="D7" s="165">
+        <v>0</v>
+      </c>
+      <c r="E7" s="165">
+        <v>0</v>
+      </c>
+      <c r="F7" s="165">
+        <v>77</v>
+      </c>
+      <c r="G7" s="165">
+        <v>46.3</v>
+      </c>
+      <c r="H7" s="165">
+        <v>86.1</v>
+      </c>
+      <c r="I7" s="165">
+        <v>2349</v>
+      </c>
+      <c r="J7" s="165">
+        <v>75</v>
+      </c>
+      <c r="K7" s="165">
+        <v>36.5</v>
+      </c>
+      <c r="L7" s="165">
+        <v>82.3</v>
+      </c>
+      <c r="M7" s="165">
+        <v>3108</v>
+      </c>
+      <c r="N7" s="165">
+        <v>292</v>
+      </c>
+      <c r="O7" s="165">
+        <v>84.6</v>
+      </c>
+      <c r="P7" s="165">
+        <v>2584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="167" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="165">
+        <v>0</v>
+      </c>
+      <c r="D8" s="165">
+        <v>0</v>
+      </c>
+      <c r="E8" s="165">
+        <v>0</v>
+      </c>
+      <c r="F8" s="165">
+        <v>4559</v>
+      </c>
+      <c r="G8" s="165">
+        <v>50.3</v>
+      </c>
+      <c r="H8" s="165">
+        <v>74.5</v>
+      </c>
+      <c r="I8" s="165">
+        <v>5025</v>
+      </c>
+      <c r="J8" s="165">
+        <v>1540</v>
+      </c>
+      <c r="K8" s="165">
+        <v>45.1</v>
+      </c>
+      <c r="L8" s="165">
+        <v>73.2</v>
+      </c>
+      <c r="M8" s="165">
+        <v>4875</v>
+      </c>
+      <c r="N8" s="165">
+        <v>1876</v>
+      </c>
+      <c r="O8" s="165">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="P8" s="165">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="167" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="165">
+        <v>39</v>
+      </c>
+      <c r="D9" s="165">
+        <v>45.6</v>
+      </c>
+      <c r="E9" s="165">
+        <v>1891</v>
+      </c>
+      <c r="F9" s="165">
+        <v>227</v>
+      </c>
+      <c r="G9" s="165">
+        <v>52.9</v>
+      </c>
+      <c r="H9" s="165">
+        <v>60.3</v>
+      </c>
+      <c r="I9" s="165">
+        <v>2888</v>
+      </c>
+      <c r="J9" s="165">
+        <v>249</v>
+      </c>
+      <c r="K9" s="165">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="L9" s="165">
+        <v>56.1</v>
+      </c>
+      <c r="M9" s="165">
+        <v>3522</v>
+      </c>
+      <c r="N9" s="165">
+        <v>83</v>
+      </c>
+      <c r="O9" s="165">
+        <v>53.3</v>
+      </c>
+      <c r="P9" s="165">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="167" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="165">
+        <v>0</v>
+      </c>
+      <c r="D10" s="165">
+        <v>0</v>
+      </c>
+      <c r="E10" s="165">
+        <v>0</v>
+      </c>
+      <c r="F10" s="165">
+        <v>202</v>
+      </c>
+      <c r="G10" s="165">
+        <v>46.5</v>
+      </c>
+      <c r="H10" s="165">
+        <v>54.3</v>
+      </c>
+      <c r="I10" s="165">
+        <v>4745</v>
+      </c>
+      <c r="J10" s="165">
+        <v>45</v>
+      </c>
+      <c r="K10" s="165">
+        <v>42.2</v>
+      </c>
+      <c r="L10" s="165">
+        <v>53.4</v>
+      </c>
+      <c r="M10" s="165">
+        <v>4525</v>
+      </c>
+      <c r="N10" s="165">
+        <v>4</v>
+      </c>
+      <c r="O10" s="165">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="P10" s="165">
+        <v>6803</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="167" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="165">
+        <v>47</v>
+      </c>
+      <c r="D11" s="165">
+        <v>47.4</v>
+      </c>
+      <c r="E11" s="165">
+        <v>4052</v>
+      </c>
+      <c r="F11" s="165">
+        <v>3046</v>
+      </c>
+      <c r="G11" s="165">
+        <v>54.2</v>
+      </c>
+      <c r="H11" s="165">
+        <v>63.7</v>
+      </c>
+      <c r="I11" s="165">
+        <v>7391</v>
+      </c>
+      <c r="J11" s="165">
+        <v>120</v>
+      </c>
+      <c r="K11" s="165">
+        <v>43.6</v>
+      </c>
+      <c r="L11" s="165">
+        <v>50.9</v>
+      </c>
+      <c r="M11" s="165">
+        <v>4745</v>
+      </c>
+      <c r="N11" s="165">
+        <v>185</v>
+      </c>
+      <c r="O11" s="165">
+        <v>54.5</v>
+      </c>
+      <c r="P11" s="165">
+        <v>5504</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="167" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="165">
+        <v>0</v>
+      </c>
+      <c r="D12" s="165">
+        <v>0</v>
+      </c>
+      <c r="E12" s="165">
+        <v>0</v>
+      </c>
+      <c r="F12" s="165">
+        <v>11</v>
+      </c>
+      <c r="G12" s="165">
+        <v>54.8</v>
+      </c>
+      <c r="H12" s="165">
+        <v>59.6</v>
+      </c>
+      <c r="I12" s="165">
+        <v>6397</v>
+      </c>
+      <c r="J12" s="165">
+        <v>2</v>
+      </c>
+      <c r="K12" s="165">
+        <v>40.1</v>
+      </c>
+      <c r="L12" s="165">
+        <v>50.1</v>
+      </c>
+      <c r="M12" s="165">
+        <v>4914</v>
+      </c>
+      <c r="N12" s="165">
+        <v>0</v>
+      </c>
+      <c r="O12" s="165">
+        <v>0</v>
+      </c>
+      <c r="P12" s="165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="167" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="166">
+        <v>26</v>
+      </c>
+      <c r="D13" s="166">
+        <v>0</v>
+      </c>
+      <c r="E13" s="166">
+        <v>0</v>
+      </c>
+      <c r="F13" s="166">
+        <v>0</v>
+      </c>
+      <c r="G13" s="166">
+        <v>0</v>
+      </c>
+      <c r="H13" s="166">
+        <v>0</v>
+      </c>
+      <c r="I13" s="166">
+        <v>0</v>
+      </c>
+      <c r="J13" s="166">
+        <v>0</v>
+      </c>
+      <c r="K13" s="166">
+        <v>0</v>
+      </c>
+      <c r="L13" s="166">
+        <v>0</v>
+      </c>
+      <c r="M13" s="166">
+        <v>0</v>
+      </c>
+      <c r="N13" s="166">
+        <v>0</v>
+      </c>
+      <c r="O13" s="166">
+        <v>0</v>
+      </c>
+      <c r="P13" s="166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="167" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" s="165">
+        <v>0</v>
+      </c>
+      <c r="D14" s="165">
+        <v>0</v>
+      </c>
+      <c r="E14" s="165">
+        <v>0</v>
+      </c>
+      <c r="F14" s="165">
+        <v>0</v>
+      </c>
+      <c r="G14" s="165">
+        <v>0</v>
+      </c>
+      <c r="H14" s="165">
+        <v>0</v>
+      </c>
+      <c r="I14" s="165">
+        <v>0</v>
+      </c>
+      <c r="J14" s="165">
+        <v>0</v>
+      </c>
+      <c r="K14" s="165">
+        <v>0</v>
+      </c>
+      <c r="L14" s="165">
+        <v>0</v>
+      </c>
+      <c r="M14" s="165">
+        <v>0</v>
+      </c>
+      <c r="N14" s="165">
+        <v>0</v>
+      </c>
+      <c r="O14" s="165">
+        <v>0</v>
+      </c>
+      <c r="P14" s="165">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add distribution of non-actives provided by LAFPP
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="11" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="16" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -27,6 +27,9 @@
     <sheet name="Other_t5_HPP" sheetId="16" r:id="rId18"/>
     <sheet name="Other_t6_HPP" sheetId="17" r:id="rId19"/>
     <sheet name="nonActives_allTiers" sheetId="22" r:id="rId20"/>
+    <sheet name="Retirees_allTiers" sheetId="23" r:id="rId21"/>
+    <sheet name="Beneficiaries_allTiers" sheetId="24" r:id="rId22"/>
+    <sheet name="Disability_allTiers" sheetId="25" r:id="rId23"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,8 +40,182 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="O6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="R3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nearest age at June 30, 2015.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="156">
   <si>
     <t>TOC</t>
   </si>
@@ -663,17 +840,84 @@
   <si>
     <t>P14</t>
   </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>NUMBER OF MEMBERS</t>
+  </si>
+  <si>
+    <t>AVERAGE BENEFIT PAYMENT</t>
+  </si>
+  <si>
+    <t>Under 45</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>75-79</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>90 &amp; over</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>benperiod</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>name_N</t>
+  </si>
+  <si>
+    <t>nretirees</t>
+  </si>
+  <si>
+    <t>name_V</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>90-94</t>
+  </si>
+  <si>
+    <t>n.R0S1</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>ndisb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,6 +1004,24 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -904,7 +1166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1376,12 +1638,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1395,6 +1651,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2792,8 +3060,8 @@
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
-      <c r="U7" s="161"/>
-      <c r="V7" s="161"/>
+      <c r="U7" s="166"/>
+      <c r="V7" s="166"/>
       <c r="W7" s="12"/>
       <c r="X7" s="109"/>
       <c r="Y7" s="109"/>
@@ -6847,7 +7115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6879,425 +7147,425 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="24" x14ac:dyDescent="0.25">
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="161" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="164" t="s">
+      <c r="C6" s="162" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="164" t="s">
+      <c r="D6" s="162" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="164" t="s">
+      <c r="E6" s="162" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="164" t="s">
+      <c r="F6" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="164" t="s">
+      <c r="I6" s="162" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="164" t="s">
+      <c r="J6" s="162" t="s">
         <v>69</v>
       </c>
-      <c r="K6" s="164" t="s">
+      <c r="K6" s="162" t="s">
         <v>70</v>
       </c>
-      <c r="L6" s="164" t="s">
+      <c r="L6" s="162" t="s">
         <v>71</v>
       </c>
-      <c r="M6" s="164" t="s">
+      <c r="M6" s="162" t="s">
         <v>72</v>
       </c>
-      <c r="N6" s="164" t="s">
+      <c r="N6" s="162" t="s">
         <v>110</v>
       </c>
-      <c r="O6" s="164" t="s">
+      <c r="O6" s="162" t="s">
         <v>111</v>
       </c>
-      <c r="P6" s="164" t="s">
+      <c r="P6" s="162" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="167" t="s">
+      <c r="B7" s="165" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="165">
+      <c r="C7" s="163">
         <v>0</v>
       </c>
-      <c r="D7" s="165">
+      <c r="D7" s="163">
         <v>0</v>
       </c>
-      <c r="E7" s="165">
+      <c r="E7" s="163">
         <v>0</v>
       </c>
-      <c r="F7" s="165">
+      <c r="F7" s="163">
         <v>77</v>
       </c>
-      <c r="G7" s="165">
+      <c r="G7" s="163">
         <v>46.3</v>
       </c>
-      <c r="H7" s="165">
+      <c r="H7" s="163">
         <v>86.1</v>
       </c>
-      <c r="I7" s="165">
+      <c r="I7" s="163">
         <v>2349</v>
       </c>
-      <c r="J7" s="165">
+      <c r="J7" s="163">
         <v>75</v>
       </c>
-      <c r="K7" s="165">
+      <c r="K7" s="163">
         <v>36.5</v>
       </c>
-      <c r="L7" s="165">
+      <c r="L7" s="163">
         <v>82.3</v>
       </c>
-      <c r="M7" s="165">
+      <c r="M7" s="163">
         <v>3108</v>
       </c>
-      <c r="N7" s="165">
+      <c r="N7" s="163">
         <v>292</v>
       </c>
-      <c r="O7" s="165">
+      <c r="O7" s="163">
         <v>84.6</v>
       </c>
-      <c r="P7" s="165">
+      <c r="P7" s="163">
         <v>2584</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="167" t="s">
+      <c r="B8" s="165" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="165">
+      <c r="C8" s="163">
         <v>0</v>
       </c>
-      <c r="D8" s="165">
+      <c r="D8" s="163">
         <v>0</v>
       </c>
-      <c r="E8" s="165">
+      <c r="E8" s="163">
         <v>0</v>
       </c>
-      <c r="F8" s="165">
+      <c r="F8" s="163">
         <v>4559</v>
       </c>
-      <c r="G8" s="165">
+      <c r="G8" s="163">
         <v>50.3</v>
       </c>
-      <c r="H8" s="165">
+      <c r="H8" s="163">
         <v>74.5</v>
       </c>
-      <c r="I8" s="165">
+      <c r="I8" s="163">
         <v>5025</v>
       </c>
-      <c r="J8" s="165">
+      <c r="J8" s="163">
         <v>1540</v>
       </c>
-      <c r="K8" s="165">
+      <c r="K8" s="163">
         <v>45.1</v>
       </c>
-      <c r="L8" s="165">
+      <c r="L8" s="163">
         <v>73.2</v>
       </c>
-      <c r="M8" s="165">
+      <c r="M8" s="163">
         <v>4875</v>
       </c>
-      <c r="N8" s="165">
+      <c r="N8" s="163">
         <v>1876</v>
       </c>
-      <c r="O8" s="165">
+      <c r="O8" s="163">
         <v>78.599999999999994</v>
       </c>
-      <c r="P8" s="165">
+      <c r="P8" s="163">
         <v>4288</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="167" t="s">
+      <c r="B9" s="165" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="165">
+      <c r="C9" s="163">
         <v>39</v>
       </c>
-      <c r="D9" s="165">
+      <c r="D9" s="163">
         <v>45.6</v>
       </c>
-      <c r="E9" s="165">
+      <c r="E9" s="163">
         <v>1891</v>
       </c>
-      <c r="F9" s="165">
+      <c r="F9" s="163">
         <v>227</v>
       </c>
-      <c r="G9" s="165">
+      <c r="G9" s="163">
         <v>52.9</v>
       </c>
-      <c r="H9" s="165">
+      <c r="H9" s="163">
         <v>60.3</v>
       </c>
-      <c r="I9" s="165">
+      <c r="I9" s="163">
         <v>2888</v>
       </c>
-      <c r="J9" s="165">
+      <c r="J9" s="163">
         <v>249</v>
       </c>
-      <c r="K9" s="165">
+      <c r="K9" s="163">
         <v>39.799999999999997</v>
       </c>
-      <c r="L9" s="165">
+      <c r="L9" s="163">
         <v>56.1</v>
       </c>
-      <c r="M9" s="165">
+      <c r="M9" s="163">
         <v>3522</v>
       </c>
-      <c r="N9" s="165">
+      <c r="N9" s="163">
         <v>83</v>
       </c>
-      <c r="O9" s="165">
+      <c r="O9" s="163">
         <v>53.3</v>
       </c>
-      <c r="P9" s="165">
+      <c r="P9" s="163">
         <v>3880</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="167" t="s">
+      <c r="B10" s="165" t="s">
         <v>119</v>
       </c>
-      <c r="C10" s="165">
+      <c r="C10" s="163">
         <v>0</v>
       </c>
-      <c r="D10" s="165">
+      <c r="D10" s="163">
         <v>0</v>
       </c>
-      <c r="E10" s="165">
+      <c r="E10" s="163">
         <v>0</v>
       </c>
-      <c r="F10" s="165">
+      <c r="F10" s="163">
         <v>202</v>
       </c>
-      <c r="G10" s="165">
+      <c r="G10" s="163">
         <v>46.5</v>
       </c>
-      <c r="H10" s="165">
+      <c r="H10" s="163">
         <v>54.3</v>
       </c>
-      <c r="I10" s="165">
+      <c r="I10" s="163">
         <v>4745</v>
       </c>
-      <c r="J10" s="165">
+      <c r="J10" s="163">
         <v>45</v>
       </c>
-      <c r="K10" s="165">
+      <c r="K10" s="163">
         <v>42.2</v>
       </c>
-      <c r="L10" s="165">
+      <c r="L10" s="163">
         <v>53.4</v>
       </c>
-      <c r="M10" s="165">
+      <c r="M10" s="163">
         <v>4525</v>
       </c>
-      <c r="N10" s="165">
+      <c r="N10" s="163">
         <v>4</v>
       </c>
-      <c r="O10" s="165">
+      <c r="O10" s="163">
         <v>35.200000000000003</v>
       </c>
-      <c r="P10" s="165">
+      <c r="P10" s="163">
         <v>6803</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="167" t="s">
+      <c r="B11" s="165" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="165">
+      <c r="C11" s="163">
         <v>47</v>
       </c>
-      <c r="D11" s="165">
+      <c r="D11" s="163">
         <v>47.4</v>
       </c>
-      <c r="E11" s="165">
+      <c r="E11" s="163">
         <v>4052</v>
       </c>
-      <c r="F11" s="165">
+      <c r="F11" s="163">
         <v>3046</v>
       </c>
-      <c r="G11" s="165">
+      <c r="G11" s="163">
         <v>54.2</v>
       </c>
-      <c r="H11" s="165">
+      <c r="H11" s="163">
         <v>63.7</v>
       </c>
-      <c r="I11" s="165">
+      <c r="I11" s="163">
         <v>7391</v>
       </c>
-      <c r="J11" s="165">
+      <c r="J11" s="163">
         <v>120</v>
       </c>
-      <c r="K11" s="165">
+      <c r="K11" s="163">
         <v>43.6</v>
       </c>
-      <c r="L11" s="165">
+      <c r="L11" s="163">
         <v>50.9</v>
       </c>
-      <c r="M11" s="165">
+      <c r="M11" s="163">
         <v>4745</v>
       </c>
-      <c r="N11" s="165">
+      <c r="N11" s="163">
         <v>185</v>
       </c>
-      <c r="O11" s="165">
+      <c r="O11" s="163">
         <v>54.5</v>
       </c>
-      <c r="P11" s="165">
+      <c r="P11" s="163">
         <v>5504</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="167" t="s">
+      <c r="B12" s="165" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="165">
+      <c r="C12" s="163">
         <v>0</v>
       </c>
-      <c r="D12" s="165">
+      <c r="D12" s="163">
         <v>0</v>
       </c>
-      <c r="E12" s="165">
+      <c r="E12" s="163">
         <v>0</v>
       </c>
-      <c r="F12" s="165">
+      <c r="F12" s="163">
         <v>11</v>
       </c>
-      <c r="G12" s="165">
+      <c r="G12" s="163">
         <v>54.8</v>
       </c>
-      <c r="H12" s="165">
+      <c r="H12" s="163">
         <v>59.6</v>
       </c>
-      <c r="I12" s="165">
+      <c r="I12" s="163">
         <v>6397</v>
       </c>
-      <c r="J12" s="165">
+      <c r="J12" s="163">
         <v>2</v>
       </c>
-      <c r="K12" s="165">
+      <c r="K12" s="163">
         <v>40.1</v>
       </c>
-      <c r="L12" s="165">
+      <c r="L12" s="163">
         <v>50.1</v>
       </c>
-      <c r="M12" s="165">
+      <c r="M12" s="163">
         <v>4914</v>
       </c>
-      <c r="N12" s="165">
+      <c r="N12" s="163">
         <v>0</v>
       </c>
-      <c r="O12" s="165">
+      <c r="O12" s="163">
         <v>0</v>
       </c>
-      <c r="P12" s="165">
+      <c r="P12" s="163">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="167" t="s">
+      <c r="B13" s="165" t="s">
         <v>131</v>
       </c>
-      <c r="C13" s="166">
+      <c r="C13" s="164">
         <v>26</v>
       </c>
-      <c r="D13" s="166">
+      <c r="D13" s="164">
         <v>0</v>
       </c>
-      <c r="E13" s="166">
+      <c r="E13" s="164">
         <v>0</v>
       </c>
-      <c r="F13" s="166">
+      <c r="F13" s="164">
         <v>0</v>
       </c>
-      <c r="G13" s="166">
+      <c r="G13" s="164">
         <v>0</v>
       </c>
-      <c r="H13" s="166">
+      <c r="H13" s="164">
         <v>0</v>
       </c>
-      <c r="I13" s="166">
+      <c r="I13" s="164">
         <v>0</v>
       </c>
-      <c r="J13" s="166">
+      <c r="J13" s="164">
         <v>0</v>
       </c>
-      <c r="K13" s="166">
+      <c r="K13" s="164">
         <v>0</v>
       </c>
-      <c r="L13" s="166">
+      <c r="L13" s="164">
         <v>0</v>
       </c>
-      <c r="M13" s="166">
+      <c r="M13" s="164">
         <v>0</v>
       </c>
-      <c r="N13" s="166">
+      <c r="N13" s="164">
         <v>0</v>
       </c>
-      <c r="O13" s="166">
+      <c r="O13" s="164">
         <v>0</v>
       </c>
-      <c r="P13" s="166">
+      <c r="P13" s="164">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="165" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="165">
+      <c r="C14" s="163">
         <v>0</v>
       </c>
-      <c r="D14" s="165">
+      <c r="D14" s="163">
         <v>0</v>
       </c>
-      <c r="E14" s="165">
+      <c r="E14" s="163">
         <v>0</v>
       </c>
-      <c r="F14" s="165">
+      <c r="F14" s="163">
         <v>0</v>
       </c>
-      <c r="G14" s="165">
+      <c r="G14" s="163">
         <v>0</v>
       </c>
-      <c r="H14" s="165">
+      <c r="H14" s="163">
         <v>0</v>
       </c>
-      <c r="I14" s="165">
+      <c r="I14" s="163">
         <v>0</v>
       </c>
-      <c r="J14" s="165">
+      <c r="J14" s="163">
         <v>0</v>
       </c>
-      <c r="K14" s="165">
+      <c r="K14" s="163">
         <v>0</v>
       </c>
-      <c r="L14" s="165">
+      <c r="L14" s="163">
         <v>0</v>
       </c>
-      <c r="M14" s="165">
+      <c r="M14" s="163">
         <v>0</v>
       </c>
-      <c r="N14" s="165">
+      <c r="N14" s="163">
         <v>0</v>
       </c>
-      <c r="O14" s="165">
+      <c r="O14" s="163">
         <v>0</v>
       </c>
-      <c r="P14" s="165">
+      <c r="P14" s="163">
         <v>0</v>
       </c>
     </row>
@@ -7307,6 +7575,1053 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="17" max="17" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="O6" s="168" t="s">
+        <v>134</v>
+      </c>
+      <c r="P6" s="168" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q6" s="168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O7" s="169" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="170">
+        <v>3885.61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="168" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="168" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="168" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="168" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="170">
+        <v>4367.6000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="169" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="169">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="171">
+        <v>3885.61</v>
+      </c>
+      <c r="O9" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9">
+        <v>224</v>
+      </c>
+      <c r="Q9" s="170">
+        <v>4958.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="169">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10" s="171">
+        <v>4367.6000000000004</v>
+      </c>
+      <c r="O10" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="P10">
+        <v>924</v>
+      </c>
+      <c r="Q10" s="170">
+        <v>6255.31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="169">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>224</v>
+      </c>
+      <c r="E11" s="171">
+        <v>4958.87</v>
+      </c>
+      <c r="O11" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11">
+        <v>1296</v>
+      </c>
+      <c r="Q11" s="170">
+        <v>6589.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="169">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <v>924</v>
+      </c>
+      <c r="E12" s="171">
+        <v>6255.31</v>
+      </c>
+      <c r="O12" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="P12">
+        <v>1931</v>
+      </c>
+      <c r="Q12" s="170">
+        <v>6304.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="169">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>1296</v>
+      </c>
+      <c r="E13" s="171">
+        <v>6589.82</v>
+      </c>
+      <c r="O13" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="P13">
+        <v>1595</v>
+      </c>
+      <c r="Q13" s="170">
+        <v>5645.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="169">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>1931</v>
+      </c>
+      <c r="E14" s="171">
+        <v>6304.52</v>
+      </c>
+      <c r="O14" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14">
+        <v>942</v>
+      </c>
+      <c r="Q14" s="170">
+        <v>5092.8999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="169">
+        <v>72</v>
+      </c>
+      <c r="D15">
+        <v>1595</v>
+      </c>
+      <c r="E15" s="171">
+        <v>5645.75</v>
+      </c>
+      <c r="O15" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="P15">
+        <v>517</v>
+      </c>
+      <c r="Q15" s="170">
+        <v>4919.8500000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="169">
+        <v>77</v>
+      </c>
+      <c r="D16">
+        <v>942</v>
+      </c>
+      <c r="E16" s="171">
+        <v>5092.8999999999996</v>
+      </c>
+      <c r="O16" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="P16">
+        <v>320</v>
+      </c>
+      <c r="Q16" s="170">
+        <v>4892.3599999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="169">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>517</v>
+      </c>
+      <c r="E17" s="171">
+        <v>4919.8500000000004</v>
+      </c>
+      <c r="O17" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="P17">
+        <v>346</v>
+      </c>
+      <c r="Q17" s="170">
+        <v>4776.54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="169">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>320</v>
+      </c>
+      <c r="E18" s="171">
+        <v>4892.3599999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="169" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="169">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>346</v>
+      </c>
+      <c r="E19" s="171">
+        <v>4776.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="20" max="20" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="168" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="168" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="168" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="168" t="s">
+        <v>151</v>
+      </c>
+      <c r="R8" s="168" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8" s="168" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" s="168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="169" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="169">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>59</v>
+      </c>
+      <c r="E9" s="171">
+        <v>4806.79</v>
+      </c>
+      <c r="R9" s="169" t="s">
+        <v>137</v>
+      </c>
+      <c r="S9">
+        <v>59</v>
+      </c>
+      <c r="T9" s="170">
+        <v>4806.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="169">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+      <c r="E10" s="171">
+        <v>4606.7700000000004</v>
+      </c>
+      <c r="R10" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10">
+        <v>29</v>
+      </c>
+      <c r="T10" s="170">
+        <v>4606.7700000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="169">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>61</v>
+      </c>
+      <c r="E11" s="171">
+        <v>4922.04</v>
+      </c>
+      <c r="R11" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11">
+        <v>61</v>
+      </c>
+      <c r="T11" s="170">
+        <v>4922.04</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="169">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <v>83</v>
+      </c>
+      <c r="E12" s="171">
+        <v>4406.47</v>
+      </c>
+      <c r="R12" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="S12">
+        <v>83</v>
+      </c>
+      <c r="T12" s="170">
+        <v>4406.47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="169">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>141</v>
+      </c>
+      <c r="E13" s="171">
+        <v>4471.72</v>
+      </c>
+      <c r="R13" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="S13">
+        <v>141</v>
+      </c>
+      <c r="T13" s="170">
+        <v>4471.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="169">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>274</v>
+      </c>
+      <c r="E14" s="171">
+        <v>4167.93</v>
+      </c>
+      <c r="R14" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14">
+        <v>274</v>
+      </c>
+      <c r="T14" s="170">
+        <v>4167.93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="169">
+        <v>72</v>
+      </c>
+      <c r="D15">
+        <v>324</v>
+      </c>
+      <c r="E15" s="171">
+        <v>4138.84</v>
+      </c>
+      <c r="R15" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="S15">
+        <v>324</v>
+      </c>
+      <c r="T15" s="170">
+        <v>4138.84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="169">
+        <v>77</v>
+      </c>
+      <c r="D16">
+        <v>309</v>
+      </c>
+      <c r="E16" s="171">
+        <v>4111.1499999999996</v>
+      </c>
+      <c r="R16" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="S16">
+        <v>309</v>
+      </c>
+      <c r="T16" s="170">
+        <v>4111.1499999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="169">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>337</v>
+      </c>
+      <c r="E17" s="171">
+        <v>4108.16</v>
+      </c>
+      <c r="R17" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="S17">
+        <v>337</v>
+      </c>
+      <c r="T17" s="170">
+        <v>4108.16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="169">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>399</v>
+      </c>
+      <c r="E18" s="171">
+        <v>3985.68</v>
+      </c>
+      <c r="R18" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="S18">
+        <v>399</v>
+      </c>
+      <c r="T18" s="170">
+        <v>3985.68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="169" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="169">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>424</v>
+      </c>
+      <c r="E19" s="171">
+        <v>4065.94</v>
+      </c>
+      <c r="R19" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="S19">
+        <v>424</v>
+      </c>
+      <c r="T19" s="170">
+        <v>4065.94</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="R3" s="168" t="s">
+        <v>134</v>
+      </c>
+      <c r="S3" s="168" t="s">
+        <v>135</v>
+      </c>
+      <c r="T3" s="168" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="R4" s="169" t="s">
+        <v>137</v>
+      </c>
+      <c r="S4">
+        <v>38</v>
+      </c>
+      <c r="T4" s="170">
+        <v>3583.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R5" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5">
+        <v>72</v>
+      </c>
+      <c r="T5" s="170">
+        <v>3869.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R6" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6">
+        <v>106</v>
+      </c>
+      <c r="T6" s="170">
+        <v>4103.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R7" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7">
+        <v>131</v>
+      </c>
+      <c r="T7" s="170">
+        <v>4239.6499999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="168" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="168" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="168" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" s="168" t="s">
+        <v>151</v>
+      </c>
+      <c r="R8" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="S8">
+        <v>160</v>
+      </c>
+      <c r="T8" s="170">
+        <v>4397.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="169" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="169">
+        <v>42</v>
+      </c>
+      <c r="D9">
+        <v>38</v>
+      </c>
+      <c r="E9" s="171">
+        <v>3583.85</v>
+      </c>
+      <c r="R9" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9">
+        <v>386</v>
+      </c>
+      <c r="T9" s="170">
+        <v>4608.32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="169" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="169">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>72</v>
+      </c>
+      <c r="E10" s="171">
+        <v>3869.52</v>
+      </c>
+      <c r="R10" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10">
+        <v>463</v>
+      </c>
+      <c r="T10" s="170">
+        <v>4687.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="169">
+        <v>52</v>
+      </c>
+      <c r="D11">
+        <v>106</v>
+      </c>
+      <c r="E11" s="171">
+        <v>4103.21</v>
+      </c>
+      <c r="R11" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="S11">
+        <v>368</v>
+      </c>
+      <c r="T11" s="170">
+        <v>4941.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="169" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="169">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <v>131</v>
+      </c>
+      <c r="E12" s="171">
+        <v>4239.6499999999996</v>
+      </c>
+      <c r="R12" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="S12">
+        <v>180</v>
+      </c>
+      <c r="T12" s="170">
+        <v>5077</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="169" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="169">
+        <v>62</v>
+      </c>
+      <c r="D13">
+        <v>160</v>
+      </c>
+      <c r="E13" s="171">
+        <v>4397.63</v>
+      </c>
+      <c r="R13" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="S13">
+        <v>93</v>
+      </c>
+      <c r="T13" s="170">
+        <v>4893.3999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="169" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="169">
+        <v>67</v>
+      </c>
+      <c r="D14">
+        <v>386</v>
+      </c>
+      <c r="E14" s="171">
+        <v>4608.32</v>
+      </c>
+      <c r="R14" s="169" t="s">
+        <v>142</v>
+      </c>
+      <c r="S14">
+        <v>34</v>
+      </c>
+      <c r="T14" s="170">
+        <v>4539.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="169" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" s="169">
+        <v>72</v>
+      </c>
+      <c r="D15">
+        <v>463</v>
+      </c>
+      <c r="E15" s="171">
+        <v>4687.91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="169" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" s="169">
+        <v>77</v>
+      </c>
+      <c r="D16">
+        <v>368</v>
+      </c>
+      <c r="E16" s="171">
+        <v>4941.8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="169" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="169">
+        <v>82</v>
+      </c>
+      <c r="D17">
+        <v>180</v>
+      </c>
+      <c r="E17" s="171">
+        <v>5077</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="169" t="s">
+        <v>141</v>
+      </c>
+      <c r="C18" s="169">
+        <v>87</v>
+      </c>
+      <c r="D18">
+        <v>93</v>
+      </c>
+      <c r="E18" s="171">
+        <v>4893.3999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="169" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" s="169">
+        <v>92</v>
+      </c>
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19" s="171">
+        <v>4539.22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9068,8 +10383,8 @@
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
-      <c r="V7" s="161"/>
-      <c r="W7" s="161"/>
+      <c r="V7" s="166"/>
+      <c r="W7" s="166"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
     </row>
@@ -10137,8 +11452,8 @@
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
-      <c r="T6" s="161"/>
-      <c r="U6" s="161"/>
+      <c r="T6" s="166"/>
+      <c r="U6" s="166"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
     </row>
@@ -11254,8 +12569,8 @@
       <c r="U7" s="109"/>
       <c r="V7" s="109"/>
       <c r="W7" s="109"/>
-      <c r="X7" s="162"/>
-      <c r="Y7" s="162"/>
+      <c r="X7" s="167"/>
+      <c r="Y7" s="167"/>
       <c r="Z7" s="109"/>
       <c r="AA7" s="109"/>
       <c r="AB7" s="109"/>

</xml_diff>

<commit_message>
update: initial unrecognized returns and adjusment for initial amortization payments
</commit_message>
<xml_diff>
--- a/Data_inputs/LAFPP_MemberData.xlsx
+++ b/Data_inputs/LAFPP_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="16" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="nonActives_allTiers" sheetId="22" r:id="rId20"/>
     <sheet name="Retirees_allTiers" sheetId="23" r:id="rId21"/>
     <sheet name="Beneficiaries_allTiers" sheetId="24" r:id="rId22"/>
-    <sheet name="Disability_allTiers" sheetId="25" r:id="rId23"/>
+    <sheet name="Disb_allTiers" sheetId="25" r:id="rId23"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -898,13 +898,13 @@
     <t>90-94</t>
   </si>
   <si>
-    <t>n.R0S1</t>
-  </si>
-  <si>
     <t>E19</t>
   </si>
   <si>
     <t>ndisb</t>
+  </si>
+  <si>
+    <t>nbeneficiaries</t>
   </si>
 </sst>
 </file>
@@ -7582,7 +7582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -7611,7 +7611,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -7934,11 +7934,12 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="20" max="20" width="23.7109375" customWidth="1"/>
   </cols>
@@ -7962,7 +7963,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -7980,7 +7981,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -8282,7 +8283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -8311,7 +8312,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R3" s="168" t="s">
         <v>134</v>
@@ -8345,7 +8346,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R5" s="169" t="s">
         <v>35</v>

</xml_diff>